<commit_message>
Pusher + Roller done
</commit_message>
<xml_diff>
--- a/sfs/io.xlsx
+++ b/sfs/io.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nuno_\Documents\Faculdade\4o_ano\2o-semestre\II\trabalho_pratico\InfInd2021\sfs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\II\InfInd2021\sfs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD6D75B-675C-4677-ACF7-49A0117ABDF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4888B89-97BB-425B-84B6-C659E6D6C97C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -883,7 +883,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1181,21 +1181,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L303" sqref="L303"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L186" sqref="L186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.77734375" style="1"/>
+    <col min="1" max="2" width="8.81640625" style="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="1"/>
-    <col min="5" max="5" width="14.77734375" style="1" customWidth="1"/>
-    <col min="6" max="9" width="8.77734375" style="1"/>
-    <col min="10" max="10" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="14.81640625" style="1" customWidth="1"/>
+    <col min="6" max="9" width="8.81640625" style="1"/>
+    <col min="10" max="10" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F1" s="1" t="s">
         <v>125</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>Wi1_O_0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="41">
         <v>1</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>Wi1_O_1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="41">
         <v>1</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>Wi1_O_2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="44">
         <v>1</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>Wi1_I_0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="56">
         <v>2</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>Wo1_O_3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="59">
         <v>2</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>Wo1_O_4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="59">
         <v>2</v>
       </c>
@@ -1424,11 +1424,11 @@
         <v>Wo1</v>
       </c>
       <c r="J8" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE(H8,"_",D8,"_", F8)</f>
         <v>Wo1_I_1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="62">
         <v>2</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>Wo1_R_0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>3</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>L7_O_5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="14">
         <v>3</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>L7_O_6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="17">
         <v>3</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>L7_I_2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>4</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>R3_O_7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>4</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>R3_O_8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>4</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>R3_O_9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>4</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>R3_O_10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>R3_I_3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>4</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>R3_I_4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>4</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>R3_I_5</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>5</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>R5_O_11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>5</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>R5_O_12</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>5</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>R5_O_13</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>5</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>R5_O_14</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>5</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>R5_I_6</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>5</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>R5_I_7</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="8">
         <v>5</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>R5_I_8</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>6</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>R9_O_15</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>6</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>R9_O_16</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>6</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>R9_O_17</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>6</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>R9_O_18</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>6</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>R9_I_9</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>6</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>R9_I_10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="8">
         <v>6</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>R9_I_11</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>7</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>R8_O_19</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>7</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>R8_O_20</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>7</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>R8_O_21</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>7</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>R8_O_22</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>7</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>R8_I_12</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>7</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>R8_I_13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="8">
         <v>7</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>R8_I_14</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>8</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>R7_O_23</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>8</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>R7_O_24</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>8</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>R7_O_25</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>8</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>R7_O_26</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>8</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>R7_I_15</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>8</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>R7_I_16</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="8">
         <v>8</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>R7_I_17</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>9</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>R6_O_27</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>9</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>R6_O_28</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>9</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>R6_O_29</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>9</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>R6_O_30</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>9</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>R6_I_18</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>9</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>R6_I_19</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="8">
         <v>9</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>R6_I_20</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>10</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>R2_O_31</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>10</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>R2_O_32</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>10</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>R2_O_33</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>10</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>R2_O_34</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>10</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>R2_I_21</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>10</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>R2_I_22</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="8">
         <v>10</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>R2_I_23</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="11">
         <v>11</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>L4_O_35</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="14">
         <v>11</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>L4_O_36</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="17">
         <v>11</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>L4_I_24</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="29">
         <v>12</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>M4_O_37</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="32">
         <v>12</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>M4_O_38</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="32">
         <v>12</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>M4_O_39</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="32">
         <v>12</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>M4_O_40</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="32">
         <v>12</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>M4_O_41</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="32">
         <v>12</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>M4_O_42</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="32">
         <v>12</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>M4_O_43</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="32">
         <v>12</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>M4_O_44</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="32">
         <v>12</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>M4_O_45</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="32">
         <v>12</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>M4_I_25</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="32">
         <v>12</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>M4_I_26</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="32">
         <v>12</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>M4_I_27</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="32">
         <v>12</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>M4_I_28</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="32">
         <v>12</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>M4_I_29</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="35">
         <v>12</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>M4_I_30</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="29">
         <v>13</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>M3_O_46</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="32">
         <v>13</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>M3_O_47</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="32">
         <v>13</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>M3_O_48</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="32">
         <v>13</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>M3_O_49</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="32">
         <v>13</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>M3_O_50</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="32">
         <v>13</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>M3_O_51</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="32">
         <v>13</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>M3_O_52</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="32">
         <v>13</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>M3_O_53</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="32">
         <v>13</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>M3_O_54</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="32">
         <v>13</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>M3_I_31</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="32">
         <v>13</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>M3_I_32</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="32">
         <v>13</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>M3_I_33</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="32">
         <v>13</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>M3_I_34</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="32">
         <v>13</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>M3_I_35</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="35">
         <v>13</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>M3_I_36</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="29">
         <v>14</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>M2_O_55</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="32">
         <v>14</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>M2_O_56</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="32">
         <v>14</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>M2_O_57</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="32">
         <v>14</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>M2_O_58</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="32">
         <v>14</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>M2_O_59</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="32">
         <v>14</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>M2_O_60</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="32">
         <v>14</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>M2_O_61</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="32">
         <v>14</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>M2_O_62</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="32">
         <v>14</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>M2_O_63</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="32">
         <v>14</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>M2_I_37</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="32">
         <v>14</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>M2_I_38</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="32">
         <v>14</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>M2_I_39</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="32">
         <v>14</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>M2_I_40</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="32">
         <v>14</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>M2_I_41</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="35">
         <v>14</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>M2_I_42</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="29">
         <v>15</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>M1_O_64</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="32">
         <v>15</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>M1_O_65</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="32">
         <v>15</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>M1_O_66</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="32">
         <v>15</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>M1_O_67</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="32">
         <v>15</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>M1_O_68</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="32">
         <v>15</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>M1_O_69</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="32">
         <v>15</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>M1_O_70</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="32">
         <v>15</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>M1_O_71</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="32">
         <v>15</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>M1_O_72</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="32">
         <v>15</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>M1_I_43</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="32">
         <v>15</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>M1_I_44</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="32">
         <v>15</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>M1_I_45</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="32">
         <v>15</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>M1_I_46</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="32">
         <v>15</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>M1_I_47</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="35">
         <v>15</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>M1_I_48</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="11">
         <v>16</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>L2_O_73</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="14">
         <v>16</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>L2_O_74</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="17">
         <v>16</v>
       </c>
@@ -5222,7 +5222,7 @@
         <v>L2_I_49</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>17</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>R4_O_75</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="5">
         <v>17</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>R4_O_76</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="5">
         <v>17</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>R4_O_77</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="5">
         <v>17</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>R4_O_78</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="5">
         <v>17</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>R4_I_50</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="5">
         <v>17</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>R4_I_51</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="8">
         <v>17</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>R4_I_52</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="11">
         <v>18</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>L3_O_79</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="14">
         <v>18</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>L3_O_80</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="17">
         <v>18</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>L3_I_53</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="11">
         <v>19</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>L5_O_81</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="14">
         <v>19</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>L5_O_82</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="17">
         <v>19</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>L5_I_54</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="47">
         <v>20</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>P3_O_83</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="50">
         <v>20</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>P3_O_84</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="50">
         <v>20</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>P3_O_85</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="50">
         <v>20</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>P3_O_86</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="50">
         <v>20</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>P3_I_55</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="50">
         <v>20</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>P3_I_56</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="53">
         <v>20</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>P3_I_57</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="47">
         <v>21</v>
       </c>
@@ -5889,7 +5889,7 @@
         <v>P2_O_87</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="50">
         <v>21</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>P2_O_88</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="50">
         <v>21</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>P2_O_89</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="50">
         <v>21</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>P2_O_90</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="50">
         <v>21</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>P2_I_58</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="50">
         <v>21</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>P2_I_59</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="53">
         <v>21</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>P2_I_60</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="47">
         <v>22</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>P1_O_91</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="50">
         <v>22</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>P1_O_92</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="50">
         <v>22</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>P1_O_93</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="50">
         <v>22</v>
       </c>
@@ -6208,7 +6208,7 @@
         <v>P1_O_94</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="50">
         <v>22</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>P1_I_61</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="50">
         <v>22</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>P1_I_62</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="53">
         <v>22</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>P1_I_63</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="11">
         <v>23</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>L6_O_95</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="14">
         <v>23</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>L6_O_96</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="17">
         <v>23</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>L6_I_64</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="2">
         <v>24</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>R1_O_97</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>24</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>R1_O_98</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>24</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>R1_O_99</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>24</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>R1_O_100</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>24</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>R1_I_65</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>24</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>R1_I_66</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" s="8">
         <v>24</v>
       </c>
@@ -6622,7 +6622,7 @@
         <v>R1_I_67</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" s="11">
         <v>25</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>L1_O_101</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" s="14">
         <v>25</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>L1_O_102</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" s="17">
         <v>25</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>L1_I_68</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" s="20">
         <v>26</v>
       </c>
@@ -6741,14 +6741,14 @@
         <v>45</v>
       </c>
       <c r="H175" s="67" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J175" s="1" t="str">
         <f t="shared" si="19"/>
-        <v>O1_I_69</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+        <v>O3_I_69</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" s="23">
         <v>27</v>
       </c>
@@ -6773,14 +6773,14 @@
       </c>
       <c r="H176" s="67" t="str">
         <f>H175</f>
-        <v>O1</v>
+        <v>O3</v>
       </c>
       <c r="J176" s="1" t="str">
         <f t="shared" si="19"/>
-        <v>O1_I_70</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+        <v>O3_I_70</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" s="26">
         <v>28</v>
       </c>
@@ -6805,14 +6805,14 @@
       </c>
       <c r="H177" s="67" t="str">
         <f>H175</f>
-        <v>O1</v>
+        <v>O3</v>
       </c>
       <c r="J177" s="1" t="str">
         <f t="shared" si="19"/>
-        <v>O1_I_71</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+        <v>O3_I_71</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" s="20">
         <v>30</v>
       </c>
@@ -6843,7 +6843,7 @@
         <v>O2_I_72</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" s="23">
         <v>31</v>
       </c>
@@ -6875,7 +6875,7 @@
         <v>O2_I_73</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" s="26">
         <v>32</v>
       </c>
@@ -6907,7 +6907,7 @@
         <v>O2_I_74</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" s="20">
         <v>34</v>
       </c>
@@ -6931,14 +6931,14 @@
         <v>4B</v>
       </c>
       <c r="H181" s="67" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J181" s="1" t="str">
         <f t="shared" si="19"/>
-        <v>O3_I_75</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+        <v>O1_I_75</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" s="23">
         <v>35</v>
       </c>
@@ -6963,14 +6963,14 @@
       </c>
       <c r="H182" s="67" t="str">
         <f>H181</f>
-        <v>O3</v>
+        <v>O1</v>
       </c>
       <c r="J182" s="1" t="str">
         <f t="shared" si="19"/>
-        <v>O3_I_76</v>
-      </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+        <v>O1_I_76</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" s="26">
         <v>36</v>
       </c>
@@ -6995,14 +6995,14 @@
       </c>
       <c r="H183" s="67" t="str">
         <f>H182</f>
-        <v>O3</v>
+        <v>O1</v>
       </c>
       <c r="J183" s="1" t="str">
         <f t="shared" si="19"/>
-        <v>O3_I_77</v>
-      </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+        <v>O1_I_77</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" s="38">
         <v>38</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>Wi2_O_103</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" s="41">
         <v>38</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>Wi2_O_104</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" s="41">
         <v>38</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>Wi2_O_105</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" s="44">
         <v>38</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>Wi2_I_78</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" s="56">
         <v>39</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>Wo2_O_106</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" s="59">
         <v>39</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>Wo2_O_107</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" s="59">
         <v>39</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>Wo2_I_79</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" s="62">
         <v>39</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>Wo2_R_1</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" s="11">
         <v>40</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>L8_O_108</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" s="14">
         <v>40</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>L8_O_109</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" s="17">
         <v>40</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>L8_I_80</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" s="2">
         <v>41</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>R10_O_110</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" s="5">
         <v>41</v>
       </c>
@@ -7414,7 +7414,7 @@
         <v>R10_O_111</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" s="5">
         <v>41</v>
       </c>
@@ -7446,7 +7446,7 @@
         <v>R10_O_112</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" s="5">
         <v>41</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>R10_O_113</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" s="5">
         <v>41</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>R10_I_81</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" s="5">
         <v>41</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>R10_I_82</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" s="8">
         <v>41</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>R10_I_83</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" s="2">
         <v>42</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>R16_O_114</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" s="5">
         <v>42</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>R16_O_115</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" s="5">
         <v>42</v>
       </c>
@@ -7669,7 +7669,7 @@
         <v>R16_O_116</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205" s="5">
         <v>42</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>R16_O_117</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206" s="5">
         <v>42</v>
       </c>
@@ -7733,7 +7733,7 @@
         <v>R16_I_84</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A207" s="5">
         <v>42</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>R16_I_85</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208" s="8">
         <v>42</v>
       </c>
@@ -7797,7 +7797,7 @@
         <v>R16_I_86</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A209" s="2">
         <v>43</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>R15_O_118</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A210" s="5">
         <v>43</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>R15_O_119</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A211" s="5">
         <v>43</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>R15_O_120</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A212" s="5">
         <v>43</v>
       </c>
@@ -7924,7 +7924,7 @@
         <v>R15_O_121</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A213" s="5">
         <v>43</v>
       </c>
@@ -7956,7 +7956,7 @@
         <v>R15_I_87</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A214" s="5">
         <v>43</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>R15_I_88</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A215" s="8">
         <v>43</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>R15_I_89</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A216" s="2">
         <v>44</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>R14_O_122</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A217" s="5">
         <v>44</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>R14_O_123</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A218" s="5">
         <v>44</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>R14_O_124</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A219" s="5">
         <v>44</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v>R14_O_125</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A220" s="5">
         <v>44</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>R14_I_90</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A221" s="5">
         <v>44</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>R14_I_91</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A222" s="8">
         <v>44</v>
       </c>
@@ -8243,7 +8243,7 @@
         <v>R14_I_92</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A223" s="2">
         <v>45</v>
       </c>
@@ -8274,7 +8274,7 @@
         <v>R13_O_126</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A224" s="5">
         <v>45</v>
       </c>
@@ -8306,7 +8306,7 @@
         <v>R13_O_127</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A225" s="5">
         <v>45</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>R13_O_128</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A226" s="5">
         <v>45</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>R13_O_129</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A227" s="5">
         <v>45</v>
       </c>
@@ -8402,7 +8402,7 @@
         <v>R13_I_93</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A228" s="5">
         <v>45</v>
       </c>
@@ -8434,7 +8434,7 @@
         <v>R13_I_94</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A229" s="8">
         <v>45</v>
       </c>
@@ -8466,7 +8466,7 @@
         <v>R13_I_95</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A230" s="2">
         <v>46</v>
       </c>
@@ -8497,7 +8497,7 @@
         <v>R12_O_130</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A231" s="5">
         <v>46</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>R12_O_131</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A232" s="5">
         <v>46</v>
       </c>
@@ -8561,7 +8561,7 @@
         <v>R12_O_132</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A233" s="5">
         <v>46</v>
       </c>
@@ -8593,7 +8593,7 @@
         <v>R12_O_133</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A234" s="5">
         <v>46</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>R12_I_96</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A235" s="5">
         <v>46</v>
       </c>
@@ -8657,7 +8657,7 @@
         <v>R12_I_97</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A236" s="8">
         <v>46</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>R12_I_98</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A237" s="2">
         <v>47</v>
       </c>
@@ -8720,7 +8720,7 @@
         <v>R11_O_134</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A238" s="5">
         <v>47</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>R11_O_135</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A239" s="5">
         <v>47</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>R11_O_136</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A240" s="5">
         <v>47</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>R11_O_137</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A241" s="5">
         <v>47</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>R11_I_99</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A242" s="5">
         <v>47</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>R11_I_100</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A243" s="8">
         <v>47</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>R11_I_101</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A244" s="11">
         <v>48</v>
       </c>
@@ -8943,7 +8943,7 @@
         <v>L10_O_138</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A245" s="14">
         <v>48</v>
       </c>
@@ -8975,7 +8975,7 @@
         <v>L10_O_139</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A246" s="17">
         <v>48</v>
       </c>
@@ -9007,7 +9007,7 @@
         <v>L10_I_102</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A247" s="29">
         <v>49</v>
       </c>
@@ -9038,7 +9038,7 @@
         <v>M8_O_140</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A248" s="32">
         <v>49</v>
       </c>
@@ -9070,7 +9070,7 @@
         <v>M8_O_141</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A249" s="32">
         <v>49</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>M8_O_142</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A250" s="32">
         <v>49</v>
       </c>
@@ -9134,7 +9134,7 @@
         <v>M8_O_143</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A251" s="32">
         <v>49</v>
       </c>
@@ -9166,7 +9166,7 @@
         <v>M8_O_144</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A252" s="32">
         <v>49</v>
       </c>
@@ -9198,7 +9198,7 @@
         <v>M8_O_145</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A253" s="32">
         <v>49</v>
       </c>
@@ -9230,7 +9230,7 @@
         <v>M8_O_146</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A254" s="32">
         <v>49</v>
       </c>
@@ -9262,7 +9262,7 @@
         <v>M8_O_147</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A255" s="32">
         <v>49</v>
       </c>
@@ -9294,7 +9294,7 @@
         <v>M8_O_148</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A256" s="32">
         <v>49</v>
       </c>
@@ -9326,7 +9326,7 @@
         <v>M8_I_103</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A257" s="32">
         <v>49</v>
       </c>
@@ -9358,7 +9358,7 @@
         <v>M8_I_104</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A258" s="32">
         <v>49</v>
       </c>
@@ -9390,7 +9390,7 @@
         <v>M8_I_105</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A259" s="32">
         <v>49</v>
       </c>
@@ -9422,7 +9422,7 @@
         <v>M8_I_106</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A260" s="32">
         <v>49</v>
       </c>
@@ -9454,7 +9454,7 @@
         <v>M8_I_107</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A261" s="35">
         <v>49</v>
       </c>
@@ -9486,7 +9486,7 @@
         <v>M8_I_108</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A262" s="29">
         <v>50</v>
       </c>
@@ -9517,7 +9517,7 @@
         <v>M7_O_149</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A263" s="32">
         <v>50</v>
       </c>
@@ -9549,7 +9549,7 @@
         <v>M7_O_150</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A264" s="32">
         <v>50</v>
       </c>
@@ -9581,7 +9581,7 @@
         <v>M7_O_151</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A265" s="32">
         <v>50</v>
       </c>
@@ -9613,7 +9613,7 @@
         <v>M7_O_152</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A266" s="32">
         <v>50</v>
       </c>
@@ -9645,7 +9645,7 @@
         <v>M7_O_153</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A267" s="32">
         <v>50</v>
       </c>
@@ -9677,7 +9677,7 @@
         <v>M7_O_154</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A268" s="32">
         <v>50</v>
       </c>
@@ -9709,7 +9709,7 @@
         <v>M7_O_155</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A269" s="32">
         <v>50</v>
       </c>
@@ -9741,7 +9741,7 @@
         <v>M7_O_156</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A270" s="32">
         <v>50</v>
       </c>
@@ -9773,7 +9773,7 @@
         <v>M7_O_157</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A271" s="32">
         <v>50</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>M7_I_109</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A272" s="32">
         <v>50</v>
       </c>
@@ -9837,7 +9837,7 @@
         <v>M7_I_110</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A273" s="32">
         <v>50</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>M7_I_111</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A274" s="32">
         <v>50</v>
       </c>
@@ -9901,7 +9901,7 @@
         <v>M7_I_112</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A275" s="32">
         <v>50</v>
       </c>
@@ -9933,7 +9933,7 @@
         <v>M7_I_113</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A276" s="35">
         <v>50</v>
       </c>
@@ -9965,7 +9965,7 @@
         <v>M7_I_114</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A277" s="29">
         <v>51</v>
       </c>
@@ -9996,7 +9996,7 @@
         <v>M6_O_158</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A278" s="32">
         <v>51</v>
       </c>
@@ -10028,7 +10028,7 @@
         <v>M6_O_159</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A279" s="32">
         <v>51</v>
       </c>
@@ -10060,7 +10060,7 @@
         <v>M6_O_160</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A280" s="32">
         <v>51</v>
       </c>
@@ -10092,7 +10092,7 @@
         <v>M6_O_161</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A281" s="32">
         <v>51</v>
       </c>
@@ -10124,7 +10124,7 @@
         <v>M6_O_162</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A282" s="32">
         <v>51</v>
       </c>
@@ -10156,7 +10156,7 @@
         <v>M6_O_163</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A283" s="32">
         <v>51</v>
       </c>
@@ -10188,7 +10188,7 @@
         <v>M6_O_164</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A284" s="32">
         <v>51</v>
       </c>
@@ -10220,7 +10220,7 @@
         <v>M6_O_165</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A285" s="32">
         <v>51</v>
       </c>
@@ -10252,7 +10252,7 @@
         <v>M6_O_166</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A286" s="32">
         <v>51</v>
       </c>
@@ -10284,7 +10284,7 @@
         <v>M6_I_115</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A287" s="32">
         <v>51</v>
       </c>
@@ -10316,7 +10316,7 @@
         <v>M6_I_116</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A288" s="32">
         <v>51</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>M6_I_117</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A289" s="32">
         <v>51</v>
       </c>
@@ -10380,7 +10380,7 @@
         <v>M6_I_118</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A290" s="32">
         <v>51</v>
       </c>
@@ -10412,7 +10412,7 @@
         <v>M6_I_119</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A291" s="35">
         <v>51</v>
       </c>
@@ -10444,7 +10444,7 @@
         <v>M6_I_120</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A292" s="29">
         <v>52</v>
       </c>
@@ -10475,7 +10475,7 @@
         <v>M5_O_167</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A293" s="32">
         <v>52</v>
       </c>
@@ -10507,7 +10507,7 @@
         <v>M5_O_168</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A294" s="32">
         <v>52</v>
       </c>
@@ -10539,7 +10539,7 @@
         <v>M5_O_169</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A295" s="32">
         <v>52</v>
       </c>
@@ -10571,7 +10571,7 @@
         <v>M5_O_170</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A296" s="32">
         <v>52</v>
       </c>
@@ -10603,7 +10603,7 @@
         <v>M5_O_171</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A297" s="32">
         <v>52</v>
       </c>
@@ -10635,7 +10635,7 @@
         <v>M5_O_172</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A298" s="32">
         <v>52</v>
       </c>
@@ -10667,7 +10667,7 @@
         <v>M5_O_173</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A299" s="32">
         <v>52</v>
       </c>
@@ -10699,7 +10699,7 @@
         <v>M5_O_174</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A300" s="32">
         <v>52</v>
       </c>
@@ -10731,7 +10731,7 @@
         <v>M5_O_175</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A301" s="32">
         <v>52</v>
       </c>
@@ -10763,7 +10763,7 @@
         <v>M5_I_121</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A302" s="32">
         <v>52</v>
       </c>
@@ -10795,7 +10795,7 @@
         <v>M5_I_122</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A303" s="32">
         <v>52</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>M5_I_123</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A304" s="32">
         <v>52</v>
       </c>
@@ -10859,7 +10859,7 @@
         <v>M5_I_124</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A305" s="32">
         <v>52</v>
       </c>
@@ -10891,7 +10891,7 @@
         <v>M5_I_125</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A306" s="35">
         <v>52</v>
       </c>
@@ -10923,7 +10923,7 @@
         <v>M5_I_126</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A307" s="11">
         <v>53</v>
       </c>
@@ -10954,7 +10954,7 @@
         <v>L9_O_176</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A308" s="14">
         <v>53</v>
       </c>
@@ -10986,7 +10986,7 @@
         <v>L9_O_177</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A309" s="17">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
List Tools Multiple Times
</commit_message>
<xml_diff>
--- a/sfs/io.xlsx
+++ b/sfs/io.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\II\InfInd2021\sfs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4888B89-97BB-425B-84B6-C659E6D6C97C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FC0422-6B13-4660-B676-994D9AE0465E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="129">
   <si>
     <t>ART1</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>Var Name</t>
+  </si>
+  <si>
+    <t>L8:R10:R11:R12:M5:M#T1|15:M#T2|15:R12:R13:M6:M#T3|15:M#T1|15:R13:R14:?P=1?ID=1_1_1'</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -816,6 +819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,16 +841,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>204466</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>62526</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>33050</xdr:rowOff>
+      <xdr:rowOff>107755</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>58608</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>529256</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>96363</xdr:rowOff>
+      <xdr:rowOff>171068</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -869,8 +873,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9103537" y="386836"/>
-          <a:ext cx="10248367" cy="6062430"/>
+          <a:off x="8511761" y="481284"/>
+          <a:ext cx="10268142" cy="6413313"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1179,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J309"/>
+  <dimension ref="A1:AE309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L186" sqref="L186"/>
+    <sheetView tabSelected="1" topLeftCell="M11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF24" sqref="AF24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1682,7 +1686,7 @@
         <v>R3_O_10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -1714,7 +1718,7 @@
         <v>R3_I_3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>4</v>
       </c>
@@ -1746,7 +1750,7 @@
         <v>R3_I_4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>4</v>
       </c>
@@ -1777,8 +1781,11 @@
         <f t="shared" si="2"/>
         <v>R3_I_5</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="AE19" s="68" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>5</v>
       </c>
@@ -1809,7 +1816,7 @@
         <v>R5_O_11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>5</v>
       </c>
@@ -1841,7 +1848,7 @@
         <v>R5_O_12</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>5</v>
       </c>
@@ -1873,7 +1880,7 @@
         <v>R5_O_13</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>5</v>
       </c>
@@ -1905,7 +1912,7 @@
         <v>R5_O_14</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>5</v>
       </c>
@@ -1937,7 +1944,7 @@
         <v>R5_I_6</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>5</v>
       </c>
@@ -1969,7 +1976,7 @@
         <v>R5_I_7</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A26" s="8">
         <v>5</v>
       </c>
@@ -2001,7 +2008,7 @@
         <v>R5_I_8</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>6</v>
       </c>
@@ -2032,7 +2039,7 @@
         <v>R9_O_15</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>6</v>
       </c>
@@ -2064,7 +2071,7 @@
         <v>R9_O_16</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>6</v>
       </c>
@@ -2096,7 +2103,7 @@
         <v>R9_O_17</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>6</v>
       </c>
@@ -2128,7 +2135,7 @@
         <v>R9_O_18</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>6</v>
       </c>
@@ -2160,7 +2167,7 @@
         <v>R9_I_9</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>6</v>
       </c>

</xml_diff>